<commit_message>
Update: Currently S9000 and 9550 work.
</commit_message>
<xml_diff>
--- a/Working/Hornerstown S9000.xlsx
+++ b/Working/Hornerstown S9000.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wblankenship\Documents\GitHub\SPT-Builder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wblankenship\Documents\GitHub\SPT-Builder\Working\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC66696D-07A4-471C-9D0A-844F7509BE32}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22439E8C-DF48-4B68-928F-759C394DB8C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D2F1E244-0055-49E9-BA99-E37AFD162BFC}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D2F1E244-0055-49E9-BA99-E37AFD162BFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="50">
   <si>
     <t>SPARE</t>
   </si>
@@ -78,16 +78,46 @@
     <t xml:space="preserve">c31 was undefined but I deleted it for the program to create the correct number of control points. Need to put in an if statement to not create a point if the point is undefined or undef. . Etc. . . </t>
   </si>
   <si>
-    <t>67291 OCB</t>
-  </si>
-  <si>
-    <t>67292 VCB</t>
-  </si>
-  <si>
-    <t>H60-2 LBSW</t>
-  </si>
-  <si>
-    <t>H60-3 LBSW</t>
+    <t>BK 1 MW</t>
+  </si>
+  <si>
+    <t>BK 1 MVAR</t>
+  </si>
+  <si>
+    <t>BK 2 MW</t>
+  </si>
+  <si>
+    <t>BK 2 MVAR</t>
+  </si>
+  <si>
+    <t>47416 phase A amps</t>
+  </si>
+  <si>
+    <t>47416 phase B amps</t>
+  </si>
+  <si>
+    <t>47416 phase C amps</t>
+  </si>
+  <si>
+    <t>47417 phase A amps</t>
+  </si>
+  <si>
+    <t>47417 phase B amps</t>
+  </si>
+  <si>
+    <t>47417 phase C amps</t>
+  </si>
+  <si>
+    <t>DIAL IN ACCESS</t>
+  </si>
+  <si>
+    <t>I87 LBSW</t>
+  </si>
+  <si>
+    <t>NO 6 LBSW</t>
+  </si>
+  <si>
+    <t>A53 LBSW</t>
   </si>
   <si>
     <t>BK 1 VCB</t>
@@ -111,36 +141,30 @@
     <t>47416 VCB</t>
   </si>
   <si>
+    <t>CAP 1 VCB</t>
+  </si>
+  <si>
     <t>47415 VCB</t>
   </si>
   <si>
-    <t>DIAL IN ACCESS</t>
-  </si>
-  <si>
     <t>BK 1 CKT INT CI-2</t>
   </si>
   <si>
+    <t>ADAPTIVE RELAYINIG</t>
+  </si>
+  <si>
+    <t>UNDEFINED</t>
+  </si>
+  <si>
     <t xml:space="preserve">SPARE </t>
   </si>
   <si>
-    <t>I87 LBSW</t>
-  </si>
-  <si>
-    <t>NO 6 LBSW</t>
-  </si>
-  <si>
-    <t>A53 LBSW</t>
-  </si>
-  <si>
     <t>BK 1 ALRM</t>
   </si>
   <si>
     <t>BK 2 ALRM</t>
   </si>
   <si>
-    <t>CAP 1 VCB</t>
-  </si>
-  <si>
     <t>DX RELAY FAIL</t>
   </si>
   <si>
@@ -150,37 +174,13 @@
     <t xml:space="preserve">BK 1 CKT INT CI-2/SEL TRBL  </t>
   </si>
   <si>
-    <t>UNDEFINED</t>
-  </si>
-  <si>
-    <t>BK 1 MW</t>
-  </si>
-  <si>
-    <t>BK 1 MVAR</t>
-  </si>
-  <si>
-    <t>BK 2 MW</t>
-  </si>
-  <si>
-    <t>BK 2 MVAR</t>
-  </si>
-  <si>
-    <t>47416 phase A amps</t>
-  </si>
-  <si>
-    <t>47416 phase B amps</t>
-  </si>
-  <si>
-    <t>47416 phase C amps</t>
-  </si>
-  <si>
-    <t>47417 phase A amps</t>
-  </si>
-  <si>
-    <t>47417 phase B amps</t>
-  </si>
-  <si>
-    <t>47417 phase C amps</t>
+    <t>ENABLE</t>
+  </si>
+  <si>
+    <t>DISABLE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CLOSE</t>
   </si>
 </sst>
 </file>
@@ -538,7 +538,7 @@
   <dimension ref="A1:H43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,16 +551,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
         <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D1" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -568,16 +568,16 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
         <v>0</v>
@@ -585,138 +585,138 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="D4" t="s">
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
         <v>18</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
       </c>
       <c r="E7" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>49</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
       </c>
       <c r="E9" t="s">
-        <v>46</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
         <v>4</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -727,10 +727,13 @@
         <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -741,10 +744,13 @@
         <v>4</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="D12" t="s">
+        <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -755,166 +761,268 @@
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="C15" t="s">
-        <v>0</v>
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
         <v>5</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B18" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>36</v>
+      </c>
+      <c r="D23" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>44</v>
+      </c>
+      <c r="B24" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" t="s">
         <v>36</v>
       </c>
-      <c r="B24" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" t="s">
         <v>37</v>
       </c>
-      <c r="B25" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="B26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>38</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>2</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>38</v>
+      </c>
+      <c r="D28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D29" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="D30" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="C32" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="135" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>14</v>
@@ -925,7 +1033,7 @@
     </row>
     <row r="35" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="G35" s="1" t="s">
         <v>13</v>
@@ -936,37 +1044,37 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>